<commit_message>
we have a vision radius woo!
attack/move and attack coming up next

hit 'r' to toggle which side you are on...
</commit_message>
<xml_diff>
--- a/Open GL Basic Engine/Content/Red vs Blue Game.xlsx
+++ b/Open GL Basic Engine/Content/Red vs Blue Game.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>multi-select</t>
   </si>
@@ -201,13 +201,16 @@
     <t>attack(ing), firing</t>
   </si>
   <si>
-    <t>0-3</t>
-  </si>
-  <si>
-    <t>..6-9</t>
-  </si>
-  <si>
-    <t>..3-6</t>
+    <t>mostly done</t>
+  </si>
+  <si>
+    <t>genetics</t>
+  </si>
+  <si>
+    <t>side definition</t>
+  </si>
+  <si>
+    <t>vision radius</t>
   </si>
 </sst>
 </file>
@@ -322,7 +325,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -332,6 +335,7 @@
     <xf numFmtId="14" fontId="5" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -630,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -723,299 +727,352 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="4" customFormat="1"/>
-    <row r="9" spans="1:6" s="4" customFormat="1"/>
-    <row r="10" spans="1:6" s="4" customFormat="1"/>
-    <row r="11" spans="1:6" s="4" customFormat="1"/>
+    <row r="9" spans="1:6" s="7" customFormat="1">
+      <c r="A9" s="6">
+        <v>40063</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="7" customFormat="1">
+      <c r="A10" s="6">
+        <v>40065</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="7" customFormat="1">
+      <c r="A11" s="6">
+        <v>40063</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="12" spans="1:6" s="4" customFormat="1"/>
-    <row r="13" spans="1:6" s="7" customFormat="1">
-      <c r="A13" s="6">
-        <v>40063</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:6" s="4" customFormat="1">
+      <c r="A13" s="9">
+        <v>40065</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1"/>
+    <row r="15" spans="1:6" s="4" customFormat="1">
+      <c r="E15" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1">
+      <c r="F16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="4" customFormat="1">
+      <c r="F17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1"/>
+    <row r="19" spans="1:6" s="4" customFormat="1">
+      <c r="A19" s="9">
+        <v>40065</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="4" customFormat="1">
-      <c r="E14" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="7" customFormat="1">
-      <c r="A15" s="6">
-        <v>40063</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="E19" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="4" customFormat="1">
+      <c r="A20" s="9">
+        <v>40065</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="4" customFormat="1"/>
-    <row r="17" spans="1:8" s="4" customFormat="1">
-      <c r="E17" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1"/>
-    <row r="19" spans="1:8" s="4" customFormat="1">
-      <c r="E19" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
-      <c r="F20" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
-      <c r="F21" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
-      <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1"/>
-    <row r="24" spans="1:8" s="4" customFormat="1"/>
-    <row r="25" spans="1:8" s="4" customFormat="1">
-      <c r="E25" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="4" customFormat="1"/>
+    <row r="22" spans="1:6" s="4" customFormat="1"/>
+    <row r="23" spans="1:6" s="4" customFormat="1"/>
+    <row r="24" spans="1:6" s="4" customFormat="1"/>
+    <row r="25" spans="1:6" s="4" customFormat="1"/>
+    <row r="26" spans="1:6" s="4" customFormat="1"/>
+    <row r="27" spans="1:6" s="4" customFormat="1"/>
+    <row r="28" spans="1:6" s="4" customFormat="1"/>
+    <row r="29" spans="1:6" s="4" customFormat="1"/>
+    <row r="30" spans="1:6" s="4" customFormat="1"/>
+    <row r="31" spans="1:6" s="4" customFormat="1">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" s="4" customFormat="1"/>
+    <row r="33" spans="1:8" s="4" customFormat="1"/>
+    <row r="34" spans="1:8" s="4" customFormat="1">
+      <c r="A34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
-      <c r="F26" s="4" t="s">
+    <row r="35" spans="1:8" s="4" customFormat="1">
+      <c r="F35" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
-      <c r="F27" s="4" t="s">
+    <row r="36" spans="1:8" s="4" customFormat="1">
+      <c r="F36" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1">
-      <c r="F28" s="4" t="s">
+    <row r="37" spans="1:8" s="4" customFormat="1">
+      <c r="F37" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
-      <c r="F29" s="4" t="s">
+    <row r="38" spans="1:8" s="4" customFormat="1">
+      <c r="F38" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
-      <c r="F30" s="4" t="s">
+    <row r="39" spans="1:8" s="4" customFormat="1">
+      <c r="F39" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
-      <c r="G31" s="4" t="s">
+    <row r="40" spans="1:8" s="4" customFormat="1">
+      <c r="G40" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1">
-      <c r="H32" s="4" t="s">
+    <row r="41" spans="1:8" s="4" customFormat="1">
+      <c r="H41" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="5:8" s="4" customFormat="1">
-      <c r="H33" s="4" t="s">
+    <row r="42" spans="1:8" s="4" customFormat="1">
+      <c r="H42" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="5:8" s="4" customFormat="1">
-      <c r="H34" s="4" t="s">
+    <row r="43" spans="1:8" s="4" customFormat="1">
+      <c r="H43" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="5:8" s="4" customFormat="1"/>
-    <row r="36" spans="5:8" s="4" customFormat="1"/>
-    <row r="37" spans="5:8" s="4" customFormat="1"/>
-    <row r="38" spans="5:8" s="4" customFormat="1"/>
-    <row r="39" spans="5:8" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="E39" s="4" t="s">
+    <row r="44" spans="1:8" s="4" customFormat="1"/>
+    <row r="45" spans="1:8" s="4" customFormat="1"/>
+    <row r="46" spans="1:8" s="4" customFormat="1"/>
+    <row r="47" spans="1:8" s="4" customFormat="1"/>
+    <row r="48" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="E48" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="5:8" s="4" customFormat="1">
-      <c r="G40" s="4" t="s">
+    <row r="49" spans="5:7" s="4" customFormat="1">
+      <c r="G49" s="4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="5:8" s="4" customFormat="1">
-      <c r="G41" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="5:8" s="4" customFormat="1"/>
-    <row r="43" spans="5:8" s="4" customFormat="1"/>
-    <row r="44" spans="5:8" s="4" customFormat="1">
-      <c r="E44" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="5:8" s="4" customFormat="1">
-      <c r="F45" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="5:8" s="4" customFormat="1">
-      <c r="G46" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="5:8" s="4" customFormat="1">
-      <c r="G47" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="5:8" s="4" customFormat="1"/>
-    <row r="49" spans="5:7" s="4" customFormat="1">
-      <c r="F49" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="50" spans="5:7" s="4" customFormat="1">
       <c r="G50" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="5:7" s="4" customFormat="1"/>
     <row r="52" spans="5:7" s="4" customFormat="1"/>
     <row r="53" spans="5:7" s="4" customFormat="1">
+      <c r="E53" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G53" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" s="4" customFormat="1">
+      <c r="F54" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" s="4" customFormat="1">
+      <c r="G55" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" s="4" customFormat="1">
+      <c r="G56" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" s="4" customFormat="1"/>
+    <row r="58" spans="5:7" s="4" customFormat="1">
+      <c r="F58" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" s="4" customFormat="1">
+      <c r="G59" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" s="4" customFormat="1"/>
+    <row r="61" spans="5:7" s="4" customFormat="1"/>
+    <row r="62" spans="5:7" s="4" customFormat="1">
+      <c r="G62" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="5:7" s="4" customFormat="1">
-      <c r="G54" s="4" t="s">
+    <row r="63" spans="5:7" s="4" customFormat="1">
+      <c r="G63" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="5:7" s="4" customFormat="1">
-      <c r="F55" s="4" t="s">
+    <row r="64" spans="5:7" s="4" customFormat="1">
+      <c r="F64" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="G64" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="57" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="58" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="F58" s="4" t="s">
+    <row r="65" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="66" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="67" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="F67" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="60" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="61" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="62" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="63" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="E63" s="4" t="s">
+    <row r="68" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="69" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="70" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="71" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="72" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="E72" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="5:7" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="F64" s="4" t="s">
+    <row r="73" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="F73" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="66" spans="5:6" s="4" customFormat="1"/>
-    <row r="67" spans="5:6" s="4" customFormat="1"/>
-    <row r="68" spans="5:6" s="4" customFormat="1"/>
-    <row r="69" spans="5:6" s="4" customFormat="1"/>
-    <row r="70" spans="5:6" s="4" customFormat="1"/>
-    <row r="71" spans="5:6" s="4" customFormat="1"/>
-    <row r="72" spans="5:6" s="4" customFormat="1">
-      <c r="E72" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="5:6" s="4" customFormat="1">
-      <c r="F73" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="5:6" s="4" customFormat="1"/>
+    <row r="74" spans="5:6" s="4" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="75" spans="5:6" s="4" customFormat="1"/>
     <row r="76" spans="5:6" s="4" customFormat="1">
       <c r="E76" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="5:6" s="4" customFormat="1">
+      <c r="F77" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="5:6" s="4" customFormat="1"/>
+    <row r="79" spans="5:6" s="4" customFormat="1"/>
+    <row r="80" spans="5:6" s="4" customFormat="1">
+      <c r="E80" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="5:6" s="4" customFormat="1"/>
+    <row r="82" spans="5:6" s="4" customFormat="1"/>
+    <row r="83" spans="5:6" s="4" customFormat="1"/>
+    <row r="84" spans="5:6" s="4" customFormat="1"/>
+    <row r="85" spans="5:6" s="4" customFormat="1">
+      <c r="E85" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="5:6" s="4" customFormat="1"/>
-    <row r="78" spans="5:6" s="4" customFormat="1">
-      <c r="F78" s="4" t="s">
+    <row r="86" spans="5:6" s="4" customFormat="1"/>
+    <row r="87" spans="5:6" s="4" customFormat="1">
+      <c r="F87" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="5:6" s="4" customFormat="1">
-      <c r="F79" s="4" t="s">
+    <row r="88" spans="5:6" s="4" customFormat="1">
+      <c r="F88" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="5:6" s="4" customFormat="1">
-      <c r="F80" s="4" t="s">
+    <row r="89" spans="5:6" s="4" customFormat="1">
+      <c r="F89" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="6:6" s="4" customFormat="1">
-      <c r="F81" s="4" t="s">
+    <row r="90" spans="5:6" s="4" customFormat="1">
+      <c r="F90" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="6:6" s="4" customFormat="1">
-      <c r="F82" s="4" t="s">
+    <row r="91" spans="5:6" s="4" customFormat="1">
+      <c r="F91" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="6:6" s="4" customFormat="1">
-      <c r="F83" s="4" t="s">
+    <row r="92" spans="5:6" s="4" customFormat="1">
+      <c r="F92" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="6:6" s="4" customFormat="1">
-      <c r="F84" s="4" t="s">
+    <row r="93" spans="5:6" s="4" customFormat="1">
+      <c r="F93" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="6:6" s="4" customFormat="1">
-      <c r="F85" s="4" t="s">
+    <row r="94" spans="5:6" s="4" customFormat="1">
+      <c r="F94" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="6:6" s="4" customFormat="1">
-      <c r="F86" s="4" t="s">
+    <row r="95" spans="5:6" s="4" customFormat="1">
+      <c r="F95" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="6:6" s="4" customFormat="1">
-      <c r="F87" s="4" t="s">
+    <row r="96" spans="5:6" s="4" customFormat="1">
+      <c r="F96" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1030,7 +1087,7 @@
   <dimension ref="B3:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>